<commit_message>
1.07 with intent update
</commit_message>
<xml_diff>
--- a/tests/data/courses.xlsx
+++ b/tests/data/courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeming/PycharmProjects/CommunityAssistant/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3152878-E85D-754B-94DA-40BD24F44BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3972B2-0FCD-EE4E-887A-1447CF5A814A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,31 +286,7 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>你叫老王，性格固执，有高血压和心脏病史，朋友少。你的母亲今年90岁了，昨天社区医生上门为其接种了疫苗第一针，你听说疫苗会引发绝症，于是你来到居委会大吵大闹，一定要工作人员给个说法。</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>你是业主董阿姨，60岁，上海人，精明能干，不爱吃亏。最近你们小区要实施垃圾分类，居委会想在你家门口新建垃圾房，你虽然是楼组长且子女都是体制内工作人员，但你依然不愿意吃这个亏。今天居委工作人员登门对你进行劝说，但你态度强硬，决定先发制人。</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>你是业主小张，今年30岁，为人正派，是一名律师。你入住小区1年来，因为小区停车位紧张，你一直利用互联网煽动居民给居委会施加压力，要求取消固定车位。在获得部分居民的联名支持后，今天你正式来到居委会，打算利用你的专业知识好好跟工作人员理论一番。</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>你是陈奶奶，今年70岁，常年独居一人，和邻居没有交流，也没有亲戚朋友。几年前你的独生女儿死于意外事故，因为女儿生前喜欢鸽子，所以你用养鸽子的方式纪念自己的女儿。但你违规搭建的鸽棚以及鸽子的粪便、鸟叫却招来了邻居们的投诉，居委会工作人员前几天找你协商拆除鸽棚，被你拒绝。之后你一想到这个事情和自己死去的女儿就觉得委屈，今天你更是委屈的落下眼泪，于是你来到居委会。</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>你们不能欺负我一个老太婆啊，共产党应该为我们做主啊！</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>你是小区业主周爷爷，今年70岁，独居老人，消息闭塞，与邻居往来较少，性格孤僻。你没读过书，是个文盲。去年经过居民的投票，小区物业费进行了上调，但你却没有注意相关的通知，也没有参加投票。今年你去交物业费的时候，发现费用比去年高了，你很生气，径直来到居委会大吵大闹。</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>你叫小苏，今年30岁，你和你丈夫都是企业白领，没有孩子，平时很少与居委会有交集。你是一个热爱网购的女生，但网购快递送货时家里经常没有人收货，你看到其他小区都引入了快递柜而你们小区没有，于是打电话到市民热线进行投诉。</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -334,13 +310,37 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>某动迁小区物业费几十年未涨，在业委会的推动下，经过居民的民主投票，2021年度开始物业费上涨了25%，从原来的8毛涨到1块。2022年独居老人周爷爷交物业费的时候发现物业费比往年要高一点，从邻居口中得知物业费上涨了。周爷爷表示很气愤，为什么他事先不知情，找居委会理论。
+    <t>你是陈奶奶，今年70岁，常年独居一人，和邻居没有交流，也没有亲戚朋友。几年前你的独生女儿死于意外事故，因为女儿生前喜欢鸽子，所以你用养鸽子的方式纪念自己的女儿。但你违规搭建的鸽棚以及鸽子的粪便、鸟叫却招来了邻居们的投诉，居委会工作人员前几天找你协商拆除鸽棚，被你拒绝。之后你一想到这个事情和自己死去的女儿就觉得委屈，今天你更是委屈的落下眼泪，于是你来到居委会找人倾诉。</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>某商品房小区，年轻人入住率较高，快递需求量较大，但是由于工作原因无法本人签收，家里又没有老人帮忙代收，年轻人小苏希望小区引进快递柜。但是由于小区没有业委会，没有人对接快递柜的引进工作，小苏对此很不满意，于是致电12345投诉。
+接下来我来扮演小苏，而您扮演接听我电话的工作人员。</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>你叫小苏，今年30岁，你和你丈夫都是企业白领，没有孩子，平时很少与居委会有交集。最近你看到其他小区都引入了快递柜而你们小区没有，后来你得知原来是你们小区没有业委会，导致无人对接此事。你又去找居委会，居委会给出了业委会候选人名单，你强烈怀疑候选人的工作能力，认为他们也搞不定此事。你回到家后致电12345进行投诉。</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>某动迁小区物业费几十年未涨，在业委会的推动下，经过居民的民主投票，2021年度开始物业费上涨了25%，从原来的8毛涨到1块。虽然物业费上涨已经普遍征得居民投票同意，且工作人员也挨家上门做了正式通知，但周爷爷在缴纳今年的物业费后依然以事先不知情为由找到居委会理论……
 接下来我来扮演周爷爷，而您扮演接待我的工作人员。</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>某商品房小区，年轻人入住率较高，快递需求量较大，但是由于工作原因无法本人签收，家里又没有老人帮忙代收，年轻人小苏希望小区引进快递柜。但是由于小区没有业委会，没有人对接快递柜的引进工作。小苏因为平时很少与居委会打交道，所以选择直接致电12345求助。
-接下来我来扮演小苏，而您扮演接听我电话的工作人员。</t>
+    <t>你是小区业主周爷爷，今年70岁，独居老人，性格孤僻。去年经过居民的投票，小区物业费进行了上调，你当时虽然没有参加投票，但确实知道此事，并且工作人员也进行过上门告知。但你对此依然十分不满意，于是在今年缴纳物业费后，径直来到居委会大吵大闹，你一口咬定物业费上涨你不知情，且事先没人告知你。</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>你叫老王，性格固执，你的母亲今年90岁了，昨天社区医生上门为其接种了疫苗第一针，你听说疫苗会引发绝症，于是你来到居委会大吵大闹，一定要工作人员给个说法，你认为工作人员的每一句话都是骗你的。</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>你是业主董阿姨，60岁，上海人，精明能干，不爱吃亏。最近你们小区要实施垃圾分类，居委会想在你家门口新建垃圾房，你虽然是楼组长且子女都是体制内工作人员，但你依然不愿意吃这个亏。今天居委工作人员登门对你进行劝说，但你态度强硬，一定要让垃圾房建在离你家较远的地方。</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>你是业主小张，是一名律师。你入住小区1年来，因为小区停车位紧张，你一直利用互联网煽动居民给居委会施加压力，要求取消固定车位。在获得部分居民的联名支持后，今天你正式来到居委会，打算利用你的专业知识跟工作人员理论一番，一定要让居委会马上取消固定车位。</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="97" zoomScaleNormal="70" zoomScaleSheetLayoutView="97" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18"/>
@@ -803,10 +803,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>22</v>
@@ -817,10 +817,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>11</v>
@@ -831,10 +831,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>13</v>
@@ -845,13 +845,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="133" customHeight="1">
@@ -859,10 +859,10 @@
         <v>15</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>16</v>
@@ -873,10 +873,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Revert "1.07 with intent update"
This reverts commit 74ccf8fbbe49e112484014b38242d2df3bfaadd3.
</commit_message>
<xml_diff>
--- a/tests/data/courses.xlsx
+++ b/tests/data/courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeming/PycharmProjects/CommunityAssistant/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECBAF37-1BC5-D048-992A-04F4EB89C98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3972B2-0FCD-EE4E-887A-1447CF5A814A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,6 +265,9 @@
     <t>业委会工作</t>
   </si>
   <si>
+    <t>居委会不作为啊，人家小区都有快递柜的，为什么就我们小区没有？临汾小区还是先进单位了，连个快递柜也没有，怎么服务我们年轻人啊？强烈呼吁安装快递柜！！！</t>
+  </si>
+  <si>
     <t>你叫王翠花，是个四十多岁的家庭妇女。你性格小气，跟邻居关系都很差。最近你们楼栋在商议加装电梯，住一楼的你很反对这件事，因为加装电梯需要更改你家的大门。今天居委会的人再次登门对你进行劝说，你认定他们是故意欺负你。</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -311,6 +314,15 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
+    <t>某商品房小区，年轻人入住率较高，快递需求量较大，但是由于工作原因无法本人签收，家里又没有老人帮忙代收，年轻人小苏希望小区引进快递柜。但是由于小区没有业委会，没有人对接快递柜的引进工作，小苏对此很不满意，于是致电12345投诉。
+接下来我来扮演小苏，而您扮演接听我电话的工作人员。</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>你叫小苏，今年30岁，你和你丈夫都是企业白领，没有孩子，平时很少与居委会有交集。最近你看到其他小区都引入了快递柜而你们小区没有，后来你得知原来是你们小区没有业委会，导致无人对接此事。你又去找居委会，居委会给出了业委会候选人名单，你强烈怀疑候选人的工作能力，认为他们也搞不定此事。你回到家后致电12345进行投诉。</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
     <t>某动迁小区物业费几十年未涨，在业委会的推动下，经过居民的民主投票，2021年度开始物业费上涨了25%，从原来的8毛涨到1块。虽然物业费上涨已经普遍征得居民投票同意，且工作人员也挨家上门做了正式通知，但周爷爷在缴纳今年的物业费后依然以事先不知情为由找到居委会理论……
 接下来我来扮演周爷爷，而您扮演接待我的工作人员。</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -329,19 +341,6 @@
   </si>
   <si>
     <t>你是业主小张，是一名律师。你入住小区1年来，因为小区停车位紧张，你一直利用互联网煽动居民给居委会施加压力，要求取消固定车位。在获得部分居民的联名支持后，今天你正式来到居委会，打算利用你的专业知识跟工作人员理论一番，一定要让居委会马上取消固定车位。</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>你们这次选举暗箱操作，谁给你们的权力选周老师，他不符合条件，你们是只手遮天。</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>某商品房小区正在进行业委会换届改选。业主徐阿姨提出小区建立二十多年来从未召开过业主大会，认为此次选举，居委会无视业主意见而完全包办，任命不符合要求的前业委会失职人员周老师继续做业委会候选人。徐阿姨对上述说辞其实并没有实际证据，之前因为拆违工作，她一直对居委会心怀不满，于是故意在选举投票现场公开对居委会发难。
-接下来我来扮演徐阿姨，而您扮演主持投票选举的工作人员。</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>你是小区业主徐阿姨，今年68岁，国企退休职工，之前居委会强制拆除了你家的违章建筑，这让你很气愤，之后凡是居委会同意的你就反对。今天你们小区进行业委会换届改选投票，你注意到候选人中有前业委会成员周老师，你认定周老师之前有失职行为，且小区建立二十多年来从未召开过业主大会，你来到投票现场，大声向主持工作的居委工作人员发难，一定要让他下不来台！</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -745,7 +744,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="97" zoomScaleNormal="70" zoomScaleSheetLayoutView="97" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18"/>
@@ -776,7 +775,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -790,10 +789,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>8</v>
@@ -804,13 +803,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="129" customHeight="1">
@@ -818,10 +817,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>11</v>
@@ -832,10 +831,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>13</v>
@@ -846,13 +845,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="133" customHeight="1">
@@ -860,10 +859,10 @@
         <v>15</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>16</v>
@@ -874,13 +873,13 @@
         <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="68" customHeight="1">

</xml_diff>